<commit_message>
bus type coloring READY, what is left - is route point names and schemes
</commit_message>
<xml_diff>
--- a/downloads/sdasd.xlsx
+++ b/downloads/sdasd.xlsx
@@ -99,9 +99,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode=""/>
     <numFmt numFmtId="165" formatCode="[mm]:ss"/>
-    <numFmt numFmtId="166" formatCode="hh:mm"/>
+    <numFmt numFmtId="166" formatCode="[hh]:mm"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="234">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -160,8 +160,892 @@
       <name val="Sylfaen"/>
       <sz val="11.0"/>
     </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Sylfaen"/>
+      <sz val="11.0"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +1102,46 @@
         <fgColor rgb="EEECE1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="CCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="CCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00B050"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="92CE50"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="92CE50"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="95B3D7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="95B3D7"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -249,7 +1173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="234">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true">
       <alignment textRotation="90" wrapText="true" horizontal="center" vertical="center"/>
@@ -285,6 +1209,669 @@
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="11" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="25" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="36" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="41" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="42" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="44" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="45" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="46" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="47" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="48" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="49" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="50" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="51" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="52" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="53" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="54" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="55" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="56" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="57" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="58" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="59" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="60" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="61" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="62" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="63" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="64" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="65" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="66" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="67" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="68" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="69" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="70" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="71" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="72" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="73" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="74" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="75" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="76" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="77" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="78" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="79" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="80" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="81" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="82" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="83" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="84" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="85" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="86" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="87" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="88" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="89" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="90" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="91" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="92" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="93" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="94" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="95" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="96" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="97" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="98" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="99" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="100" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="101" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="102" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="103" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="104" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="105" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="106" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="107" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="108" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="109" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="110" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="111" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="112" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="113" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="114" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="115" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="116" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="117" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="118" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="119" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="120" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="121" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="122" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="123" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="124" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="125" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="126" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="127" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="128" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="129" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="130" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="131" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="132" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="133" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="134" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="135" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="136" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="137" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="138" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="139" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="140" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="141" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="142" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="143" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="144" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="145" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="146" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="147" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="148" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="149" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="150" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="151" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="152" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="153" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="154" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="155" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="156" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="157" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="158" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="159" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="160" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="161" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="162" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="163" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="164" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="165" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="166" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="167" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="168" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="169" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="170" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="171" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="172" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="173" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="174" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="175" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="176" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="177" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="178" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="179" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="180" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="181" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="182" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="183" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="184" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="185" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="186" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="187" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="188" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="189" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="190" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="191" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="192" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="193" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="194" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="195" fillId="5" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="196" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="197" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="198" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="199" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="200" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="201" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="202" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="203" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="204" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="205" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="206" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="207" fillId="19" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="208" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="209" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="210" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="211" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="212" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="213" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="214" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="215" fillId="13" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="216" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="217" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="218" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="219" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="220" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="221" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="222" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="223" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="224" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="225" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="226" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="227" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="228" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="229" fillId="17" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="230" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="231" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="232" fillId="9" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="233" fillId="15" borderId="4" xfId="0" applyFill="true" applyAlignment="true" applyBorder="true" applyFont="true" applyNumberFormat="true">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -499,7 +2086,7 @@
       <c r="C5" t="n" s="8">
         <v>1.0</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="14">
         <v>21</v>
       </c>
       <c r="G5" t="n" s="9">
@@ -517,7 +2104,9 @@
       <c r="K5" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L5"/>
+      <c r="L5" t="n" s="12">
+        <v>0.9930555555555556</v>
+      </c>
       <c r="M5" t="n" s="12">
         <v>0.9770833333333333</v>
       </c>
@@ -544,7 +2133,7 @@
       <c r="C6" t="n" s="8">
         <v>2.0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="16">
         <v>22</v>
       </c>
       <c r="G6" t="n" s="9">
@@ -562,7 +2151,9 @@
       <c r="K6" t="n" s="12">
         <v>0.28125</v>
       </c>
-      <c r="L6"/>
+      <c r="L6" t="n" s="12">
+        <v>1.007638888888889</v>
+      </c>
       <c r="M6" t="n" s="12">
         <v>0.9826388888888888</v>
       </c>
@@ -589,7 +2180,7 @@
       <c r="C7" t="n" s="8">
         <v>3.0</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" t="s" s="18">
         <v>22</v>
       </c>
       <c r="G7" t="n" s="9">
@@ -607,7 +2198,9 @@
       <c r="K7" t="n" s="12">
         <v>0.2847222222222222</v>
       </c>
-      <c r="L7"/>
+      <c r="L7" t="n" s="12">
+        <v>0.9826388888888888</v>
+      </c>
       <c r="M7" t="n" s="12">
         <v>0.9736111111111111</v>
       </c>
@@ -634,7 +2227,7 @@
       <c r="C8" t="n" s="8">
         <v>4.0</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" t="s" s="20">
         <v>23</v>
       </c>
       <c r="G8" t="n" s="9">
@@ -652,7 +2245,9 @@
       <c r="K8" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L8"/>
+      <c r="L8" t="n" s="12">
+        <v>0.9951388888888889</v>
+      </c>
       <c r="M8" t="n" s="12">
         <v>0.9840277777777777</v>
       </c>
@@ -679,7 +2274,7 @@
       <c r="C9" t="n" s="8">
         <v>5.0</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" t="s" s="22">
         <v>23</v>
       </c>
       <c r="G9" t="n" s="9">
@@ -697,7 +2292,9 @@
       <c r="K9" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L9"/>
+      <c r="L9" t="n" s="12">
+        <v>0.9770833333333333</v>
+      </c>
       <c r="M9" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
@@ -724,7 +2321,7 @@
       <c r="C10" t="n" s="8">
         <v>6.0</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" t="s" s="24">
         <v>22</v>
       </c>
       <c r="G10" t="n" s="9">
@@ -742,7 +2339,9 @@
       <c r="K10" t="n" s="12">
         <v>0.3055555555555556</v>
       </c>
-      <c r="L10"/>
+      <c r="L10" t="n" s="12">
+        <v>1.0229166666666667</v>
+      </c>
       <c r="M10" t="n" s="12">
         <v>1.0</v>
       </c>
@@ -769,7 +2368,7 @@
       <c r="C11" t="n" s="8">
         <v>7.0</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" t="s" s="26">
         <v>23</v>
       </c>
       <c r="G11" t="n" s="9">
@@ -787,7 +2386,9 @@
       <c r="K11" t="n" s="12">
         <v>0.2847222222222222</v>
       </c>
-      <c r="L11"/>
+      <c r="L11" t="n" s="12">
+        <v>0.9770833333333333</v>
+      </c>
       <c r="M11" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
@@ -814,7 +2415,7 @@
       <c r="C12" t="n" s="8">
         <v>9.0</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" t="s" s="28">
         <v>24</v>
       </c>
       <c r="G12" t="n" s="9">
@@ -832,7 +2433,9 @@
       <c r="K12" t="n" s="12">
         <v>0.2708333333333333</v>
       </c>
-      <c r="L12"/>
+      <c r="L12" t="n" s="12">
+        <v>0.9868055555555556</v>
+      </c>
       <c r="M12" t="n" s="12">
         <v>0.9736111111111111</v>
       </c>
@@ -859,7 +2462,7 @@
       <c r="C13" t="n" s="8">
         <v>10.0</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" t="s" s="30">
         <v>23</v>
       </c>
       <c r="G13" t="n" s="9">
@@ -877,7 +2480,9 @@
       <c r="K13" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L13"/>
+      <c r="L13" t="n" s="12">
+        <v>1.0263888888888888</v>
+      </c>
       <c r="M13" t="n" s="12">
         <v>0.9902777777777778</v>
       </c>
@@ -904,7 +2509,7 @@
       <c r="C14" t="n" s="8">
         <v>11.0</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" t="s" s="32">
         <v>24</v>
       </c>
       <c r="G14" t="n" s="9">
@@ -922,7 +2527,9 @@
       <c r="K14" t="n" s="12">
         <v>0.2861111111111111</v>
       </c>
-      <c r="L14"/>
+      <c r="L14" t="n" s="12">
+        <v>1.00625</v>
+      </c>
       <c r="M14" t="n" s="12">
         <v>0.9923611111111111</v>
       </c>
@@ -949,7 +2556,7 @@
       <c r="C15" t="n" s="8">
         <v>12.0</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" t="s" s="34">
         <v>23</v>
       </c>
       <c r="G15" t="n" s="9">
@@ -967,7 +2574,9 @@
       <c r="K15" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L15"/>
+      <c r="L15" t="n" s="12">
+        <v>1.0041666666666667</v>
+      </c>
       <c r="M15" t="n" s="12">
         <v>0.9909722222222223</v>
       </c>
@@ -994,7 +2603,7 @@
       <c r="C16" t="n" s="8">
         <v>14.0</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" t="s" s="36">
         <v>24</v>
       </c>
       <c r="G16" t="n" s="9">
@@ -1012,7 +2621,9 @@
       <c r="K16" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L16"/>
+      <c r="L16" t="n" s="12">
+        <v>1.0055555555555555</v>
+      </c>
       <c r="M16" t="n" s="12">
         <v>0.9958333333333333</v>
       </c>
@@ -1039,7 +2650,7 @@
       <c r="C17" t="n" s="8">
         <v>15.0</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" t="s" s="38">
         <v>24</v>
       </c>
       <c r="G17" t="n" s="9">
@@ -1057,7 +2668,9 @@
       <c r="K17" t="n" s="12">
         <v>0.2986111111111111</v>
       </c>
-      <c r="L17"/>
+      <c r="L17" t="n" s="12">
+        <v>0.9916666666666667</v>
+      </c>
       <c r="M17" t="n" s="12">
         <v>0.9791666666666666</v>
       </c>
@@ -1084,7 +2697,7 @@
       <c r="C18" t="n" s="8">
         <v>16.0</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" t="s" s="40">
         <v>23</v>
       </c>
       <c r="G18" t="n" s="9">
@@ -1102,7 +2715,9 @@
       <c r="K18" t="n" s="12">
         <v>0.3333333333333333</v>
       </c>
-      <c r="L18"/>
+      <c r="L18" t="n" s="12">
+        <v>0.9215277777777777</v>
+      </c>
       <c r="M18" t="n" s="12">
         <v>0.9166666666666666</v>
       </c>
@@ -1129,7 +2744,7 @@
       <c r="C19" t="n" s="8">
         <v>17.0</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" t="s" s="42">
         <v>22</v>
       </c>
       <c r="G19" t="n" s="9">
@@ -1147,7 +2762,9 @@
       <c r="K19" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L19"/>
+      <c r="L19" t="n" s="12">
+        <v>0.9902777777777778</v>
+      </c>
       <c r="M19" t="n" s="12">
         <v>0.9791666666666666</v>
       </c>
@@ -1174,7 +2791,7 @@
       <c r="C20" t="n" s="8">
         <v>18.0</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" t="s" s="44">
         <v>23</v>
       </c>
       <c r="G20" t="n" s="9">
@@ -1192,7 +2809,9 @@
       <c r="K20" t="n" s="12">
         <v>0.2708333333333333</v>
       </c>
-      <c r="L20"/>
+      <c r="L20" t="n" s="12">
+        <v>0.9965277777777778</v>
+      </c>
       <c r="M20" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
@@ -1219,7 +2838,7 @@
       <c r="C21" t="n" s="8">
         <v>20.0</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" t="s" s="46">
         <v>21</v>
       </c>
       <c r="G21" t="n" s="9">
@@ -1237,7 +2856,9 @@
       <c r="K21" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L21"/>
+      <c r="L21" t="n" s="12">
+        <v>1.0083333333333333</v>
+      </c>
       <c r="M21" t="n" s="12">
         <v>0.9868055555555556</v>
       </c>
@@ -1264,7 +2885,7 @@
       <c r="C22" t="n" s="8">
         <v>21.0</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" t="s" s="48">
         <v>24</v>
       </c>
       <c r="G22" t="n" s="9">
@@ -1282,7 +2903,9 @@
       <c r="K22" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L22"/>
+      <c r="L22" t="n" s="12">
+        <v>1.0208333333333333</v>
+      </c>
       <c r="M22" t="n" s="12">
         <v>1.0118055555555556</v>
       </c>
@@ -1309,7 +2932,7 @@
       <c r="C23" t="n" s="8">
         <v>22.0</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" t="s" s="50">
         <v>23</v>
       </c>
       <c r="G23" t="n" s="9">
@@ -1327,7 +2950,9 @@
       <c r="K23" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L23"/>
+      <c r="L23" t="n" s="12">
+        <v>1.0013888888888889</v>
+      </c>
       <c r="M23" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
@@ -1354,7 +2979,7 @@
       <c r="C24" t="n" s="8">
         <v>23.0</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" t="s" s="52">
         <v>24</v>
       </c>
       <c r="G24" t="n" s="9">
@@ -1372,7 +2997,9 @@
       <c r="K24" t="n" s="12">
         <v>0.3013888888888889</v>
       </c>
-      <c r="L24"/>
+      <c r="L24" t="n" s="12">
+        <v>1.007638888888889</v>
+      </c>
       <c r="M24" t="n" s="12">
         <v>0.9909722222222223</v>
       </c>
@@ -1399,7 +3026,7 @@
       <c r="C25" t="n" s="8">
         <v>24.0</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" t="s" s="54">
         <v>24</v>
       </c>
       <c r="G25" t="n" s="9">
@@ -1417,7 +3044,9 @@
       <c r="K25" t="n" s="12">
         <v>0.2986111111111111</v>
       </c>
-      <c r="L25"/>
+      <c r="L25" t="n" s="12">
+        <v>1.0131944444444445</v>
+      </c>
       <c r="M25" t="n" s="12">
         <v>0.9986111111111111</v>
       </c>
@@ -1444,7 +3073,7 @@
       <c r="C26" t="n" s="8">
         <v>25.0</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" t="s" s="56">
         <v>21</v>
       </c>
       <c r="G26" t="n" s="9">
@@ -1462,7 +3091,9 @@
       <c r="K26" t="n" s="12">
         <v>0.2743055555555556</v>
       </c>
-      <c r="L26"/>
+      <c r="L26" t="n" s="12">
+        <v>0.9881944444444445</v>
+      </c>
       <c r="M26" t="n" s="12">
         <v>0.9784722222222222</v>
       </c>
@@ -1489,7 +3120,7 @@
       <c r="C27" t="n" s="8">
         <v>26.0</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F27" t="s" s="58">
         <v>23</v>
       </c>
       <c r="G27" t="n" s="9">
@@ -1507,7 +3138,9 @@
       <c r="K27" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L27"/>
+      <c r="L27" t="n" s="12">
+        <v>0.91875</v>
+      </c>
       <c r="M27" t="n" s="12">
         <v>0.9131944444444444</v>
       </c>
@@ -1534,7 +3167,7 @@
       <c r="C28" t="n" s="8">
         <v>27.0</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F28" t="s" s="60">
         <v>23</v>
       </c>
       <c r="G28" t="n" s="9">
@@ -1552,7 +3185,9 @@
       <c r="K28" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L28"/>
+      <c r="L28" t="n" s="12">
+        <v>0.9854166666666667</v>
+      </c>
       <c r="M28" t="n" s="12">
         <v>0.9763888888888889</v>
       </c>
@@ -1579,7 +3214,7 @@
       <c r="C29" t="n" s="8">
         <v>28.0</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" t="s" s="62">
         <v>23</v>
       </c>
       <c r="G29" t="n" s="9">
@@ -1597,7 +3232,9 @@
       <c r="K29" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L29"/>
+      <c r="L29" t="n" s="12">
+        <v>0.9805555555555555</v>
+      </c>
       <c r="M29" t="n" s="12">
         <v>0.96875</v>
       </c>
@@ -1624,7 +3261,7 @@
       <c r="C30" t="n" s="8">
         <v>29.0</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" t="s" s="64">
         <v>23</v>
       </c>
       <c r="G30" t="n" s="9">
@@ -1642,7 +3279,9 @@
       <c r="K30" t="n" s="12">
         <v>0.29375</v>
       </c>
-      <c r="L30"/>
+      <c r="L30" t="n" s="12">
+        <v>0.9902777777777778</v>
+      </c>
       <c r="M30" t="n" s="12">
         <v>0.9791666666666666</v>
       </c>
@@ -1669,7 +3308,7 @@
       <c r="C31" t="n" s="8">
         <v>30.0</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" t="s" s="66">
         <v>25</v>
       </c>
       <c r="G31" t="n" s="9">
@@ -1687,7 +3326,9 @@
       <c r="K31" t="n" s="12">
         <v>0.28125</v>
       </c>
-      <c r="L31"/>
+      <c r="L31" t="n" s="12">
+        <v>0.98125</v>
+      </c>
       <c r="M31" t="n" s="12">
         <v>0.9756944444444444</v>
       </c>
@@ -1714,7 +3355,7 @@
       <c r="C32" t="n" s="8">
         <v>31.0</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" t="s" s="68">
         <v>23</v>
       </c>
       <c r="G32" t="n" s="9">
@@ -1732,7 +3373,9 @@
       <c r="K32" t="n" s="12">
         <v>0.28888888888888886</v>
       </c>
-      <c r="L32"/>
+      <c r="L32" t="n" s="12">
+        <v>0.9930555555555556</v>
+      </c>
       <c r="M32" t="n" s="12">
         <v>0.9833333333333333</v>
       </c>
@@ -1759,7 +3402,7 @@
       <c r="C33" t="n" s="8">
         <v>32.0</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" t="s" s="70">
         <v>24</v>
       </c>
       <c r="G33" t="n" s="9">
@@ -1777,7 +3420,9 @@
       <c r="K33" t="n" s="12">
         <v>0.25</v>
       </c>
-      <c r="L33"/>
+      <c r="L33" t="n" s="12">
+        <v>0.9791666666666666</v>
+      </c>
       <c r="M33" t="n" s="12">
         <v>0.96875</v>
       </c>
@@ -1804,7 +3449,7 @@
       <c r="C34" t="n" s="8">
         <v>33.0</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F34" t="s" s="72">
         <v>22</v>
       </c>
       <c r="G34" t="n" s="9">
@@ -1822,7 +3467,9 @@
       <c r="K34" t="n" s="12">
         <v>0.2951388888888889</v>
       </c>
-      <c r="L34"/>
+      <c r="L34" t="n" s="12">
+        <v>1.0069444444444444</v>
+      </c>
       <c r="M34" t="n" s="12">
         <v>0.9951388888888889</v>
       </c>
@@ -1849,7 +3496,7 @@
       <c r="C35" t="n" s="8">
         <v>34.0</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" t="s" s="74">
         <v>23</v>
       </c>
       <c r="G35" t="n" s="9">
@@ -1867,7 +3514,9 @@
       <c r="K35" t="n" s="12">
         <v>0.2673611111111111</v>
       </c>
-      <c r="L35"/>
+      <c r="L35" t="n" s="12">
+        <v>1.0138888888888888</v>
+      </c>
       <c r="M35" t="n" s="12">
         <v>0.9923611111111111</v>
       </c>
@@ -1894,7 +3543,7 @@
       <c r="C36" t="n" s="8">
         <v>35.0</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" t="s" s="76">
         <v>25</v>
       </c>
       <c r="G36" t="n" s="9">
@@ -1912,7 +3561,9 @@
       <c r="K36" t="n" s="12">
         <v>0.2708333333333333</v>
       </c>
-      <c r="L36"/>
+      <c r="L36" t="n" s="12">
+        <v>0.9513888888888888</v>
+      </c>
       <c r="M36" t="n" s="12">
         <v>0.9375</v>
       </c>
@@ -1939,7 +3590,7 @@
       <c r="C37" t="n" s="8">
         <v>36.0</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" t="s" s="78">
         <v>23</v>
       </c>
       <c r="G37" t="n" s="9">
@@ -1957,7 +3608,9 @@
       <c r="K37" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L37"/>
+      <c r="L37" t="n" s="12">
+        <v>0.9736111111111111</v>
+      </c>
       <c r="M37" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
@@ -1984,7 +3637,7 @@
       <c r="C38" t="n" s="8">
         <v>37.0</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F38" t="s" s="80">
         <v>22</v>
       </c>
       <c r="G38" t="n" s="9">
@@ -2002,7 +3655,9 @@
       <c r="K38" t="n" s="12">
         <v>0.25</v>
       </c>
-      <c r="L38"/>
+      <c r="L38" t="n" s="12">
+        <v>1.023611111111111</v>
+      </c>
       <c r="M38" t="n" s="12">
         <v>1.0</v>
       </c>
@@ -2029,7 +3684,7 @@
       <c r="C39" t="n" s="8">
         <v>38.0</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" t="s" s="82">
         <v>22</v>
       </c>
       <c r="G39" t="n" s="9">
@@ -2047,7 +3702,9 @@
       <c r="K39" t="n" s="12">
         <v>0.3194444444444444</v>
       </c>
-      <c r="L39"/>
+      <c r="L39" t="n" s="12">
+        <v>0.9819444444444444</v>
+      </c>
       <c r="M39" t="n" s="12">
         <v>0.975</v>
       </c>
@@ -2074,7 +3731,7 @@
       <c r="C40" t="n" s="8">
         <v>39.0</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F40" t="s" s="84">
         <v>21</v>
       </c>
       <c r="G40" t="n" s="9">
@@ -2092,7 +3749,9 @@
       <c r="K40" t="n" s="12">
         <v>0.2708333333333333</v>
       </c>
-      <c r="L40"/>
+      <c r="L40" t="n" s="12">
+        <v>0.9826388888888888</v>
+      </c>
       <c r="M40" t="n" s="12">
         <v>0.9729166666666667</v>
       </c>
@@ -2119,7 +3778,7 @@
       <c r="C41" t="n" s="8">
         <v>40.0</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" t="s" s="86">
         <v>23</v>
       </c>
       <c r="G41" t="n" s="9">
@@ -2137,7 +3796,9 @@
       <c r="K41" t="n" s="12">
         <v>0.3055555555555556</v>
       </c>
-      <c r="L41"/>
+      <c r="L41" t="n" s="12">
+        <v>0.9791666666666666</v>
+      </c>
       <c r="M41" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
@@ -2164,7 +3825,7 @@
       <c r="C42" t="n" s="8">
         <v>41.0</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F42" t="s" s="88">
         <v>23</v>
       </c>
       <c r="G42" t="n" s="9">
@@ -2182,7 +3843,9 @@
       <c r="K42" t="n" s="12">
         <v>0.3055555555555556</v>
       </c>
-      <c r="L42"/>
+      <c r="L42" t="n" s="12">
+        <v>1.0069444444444444</v>
+      </c>
       <c r="M42" t="n" s="12">
         <v>0.9930555555555556</v>
       </c>
@@ -2209,7 +3872,7 @@
       <c r="C43" t="n" s="8">
         <v>42.0</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F43" t="s" s="90">
         <v>23</v>
       </c>
       <c r="G43" t="n" s="9">
@@ -2227,7 +3890,9 @@
       <c r="K43" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L43"/>
+      <c r="L43" t="n" s="12">
+        <v>0.9902777777777778</v>
+      </c>
       <c r="M43" t="n" s="12">
         <v>0.9729166666666667</v>
       </c>
@@ -2254,7 +3919,7 @@
       <c r="C44" t="n" s="8">
         <v>43.0</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" t="s" s="92">
         <v>21</v>
       </c>
       <c r="G44" t="n" s="9">
@@ -2272,7 +3937,9 @@
       <c r="K44" t="n" s="12">
         <v>0.3020833333333333</v>
       </c>
-      <c r="L44"/>
+      <c r="L44" t="n" s="12">
+        <v>0.975</v>
+      </c>
       <c r="M44" t="n" s="12">
         <v>0.96875</v>
       </c>
@@ -2299,7 +3966,7 @@
       <c r="C45" t="n" s="8">
         <v>45.0</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" t="s" s="94">
         <v>23</v>
       </c>
       <c r="G45" t="n" s="9">
@@ -2317,7 +3984,9 @@
       <c r="K45" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L45"/>
+      <c r="L45" t="n" s="12">
+        <v>0.9597222222222223</v>
+      </c>
       <c r="M45" t="n" s="12">
         <v>0.9527777777777777</v>
       </c>
@@ -2344,7 +4013,7 @@
       <c r="C46" t="n" s="8">
         <v>45.099998474121094</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" t="s" s="96">
         <v>23</v>
       </c>
       <c r="G46" t="n" s="9">
@@ -2362,7 +4031,9 @@
       <c r="K46" t="n" s="12">
         <v>0.3194444444444444</v>
       </c>
-      <c r="L46"/>
+      <c r="L46" t="n" s="12">
+        <v>0.96875</v>
+      </c>
       <c r="M46" t="n" s="12">
         <v>0.9652777777777778</v>
       </c>
@@ -2389,7 +4060,7 @@
       <c r="C47" t="n" s="8">
         <v>45.20000076293945</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" t="s" s="98">
         <v>25</v>
       </c>
       <c r="G47" t="n" s="9">
@@ -2407,7 +4078,9 @@
       <c r="K47" t="n" s="12">
         <v>0.3055555555555556</v>
       </c>
-      <c r="L47"/>
+      <c r="L47" t="n" s="12">
+        <v>0.9791666666666666</v>
+      </c>
       <c r="M47" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
@@ -2434,7 +4107,7 @@
       <c r="C48" t="n" s="8">
         <v>46.0</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F48" t="s" s="100">
         <v>22</v>
       </c>
       <c r="G48" t="n" s="9">
@@ -2452,7 +4125,9 @@
       <c r="K48" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L48"/>
+      <c r="L48" t="n" s="12">
+        <v>1.0097222222222222</v>
+      </c>
       <c r="M48" t="n" s="12">
         <v>0.9916666666666667</v>
       </c>
@@ -2479,7 +4154,7 @@
       <c r="C49" t="n" s="8">
         <v>47.0</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" t="s" s="102">
         <v>23</v>
       </c>
       <c r="G49" t="n" s="9">
@@ -2497,7 +4172,9 @@
       <c r="K49" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L49"/>
+      <c r="L49" t="n" s="12">
+        <v>0.9875</v>
+      </c>
       <c r="M49" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
@@ -2524,7 +4201,7 @@
       <c r="C50" t="n" s="8">
         <v>49.0</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" t="s" s="104">
         <v>23</v>
       </c>
       <c r="G50" t="n" s="9">
@@ -2542,7 +4219,9 @@
       <c r="K50" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L50"/>
+      <c r="L50" t="n" s="12">
+        <v>0.9909722222222223</v>
+      </c>
       <c r="M50" t="n" s="12">
         <v>0.9805555555555555</v>
       </c>
@@ -2569,7 +4248,7 @@
       <c r="C51" t="n" s="8">
         <v>50.0</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" t="s" s="106">
         <v>21</v>
       </c>
       <c r="G51" t="n" s="9">
@@ -2587,7 +4266,9 @@
       <c r="K51" t="n" s="12">
         <v>0.2777777777777778</v>
       </c>
-      <c r="L51"/>
+      <c r="L51" t="n" s="12">
+        <v>0.9951388888888889</v>
+      </c>
       <c r="M51" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
@@ -2614,7 +4295,7 @@
       <c r="C52" t="n" s="8">
         <v>51.0</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" t="s" s="108">
         <v>24</v>
       </c>
       <c r="G52" t="n" s="9">
@@ -2632,7 +4313,9 @@
       <c r="K52" t="n" s="12">
         <v>0.2708333333333333</v>
       </c>
-      <c r="L52"/>
+      <c r="L52" t="n" s="12">
+        <v>1.0229166666666667</v>
+      </c>
       <c r="M52" t="n" s="12">
         <v>1.0104166666666667</v>
       </c>
@@ -2659,7 +4342,7 @@
       <c r="C53" t="n" s="8">
         <v>52.0</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" t="s" s="110">
         <v>23</v>
       </c>
       <c r="G53" t="n" s="9">
@@ -2677,7 +4360,9 @@
       <c r="K53" t="n" s="12">
         <v>0.3020833333333333</v>
       </c>
-      <c r="L53"/>
+      <c r="L53" t="n" s="12">
+        <v>0.98125</v>
+      </c>
       <c r="M53" t="n" s="12">
         <v>0.96875</v>
       </c>
@@ -2704,7 +4389,7 @@
       <c r="C54" t="n" s="8">
         <v>53.0</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" t="s" s="112">
         <v>23</v>
       </c>
       <c r="G54" t="n" s="9">
@@ -2722,7 +4407,9 @@
       <c r="K54" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L54"/>
+      <c r="L54" t="n" s="12">
+        <v>0.9875</v>
+      </c>
       <c r="M54" t="n" s="12">
         <v>0.9756944444444444</v>
       </c>
@@ -2749,7 +4436,7 @@
       <c r="C55" t="n" s="8">
         <v>54.0</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F55" t="s" s="114">
         <v>24</v>
       </c>
       <c r="G55" t="n" s="9">
@@ -2767,7 +4454,9 @@
       <c r="K55" t="n" s="12">
         <v>0.2951388888888889</v>
       </c>
-      <c r="L55"/>
+      <c r="L55" t="n" s="12">
+        <v>0.9986111111111111</v>
+      </c>
       <c r="M55" t="n" s="12">
         <v>0.9979166666666667</v>
       </c>
@@ -2794,7 +4483,7 @@
       <c r="C56" t="n" s="8">
         <v>56.0</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" t="s" s="116">
         <v>21</v>
       </c>
       <c r="G56" t="n" s="9">
@@ -2812,7 +4501,9 @@
       <c r="K56" t="n" s="12">
         <v>0.3055555555555556</v>
       </c>
-      <c r="L56"/>
+      <c r="L56" t="n" s="12">
+        <v>0.9909722222222223</v>
+      </c>
       <c r="M56" t="n" s="12">
         <v>0.9805555555555555</v>
       </c>
@@ -2839,7 +4530,7 @@
       <c r="C57" t="n" s="8">
         <v>57.0</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F57" t="s" s="118">
         <v>23</v>
       </c>
       <c r="G57" t="n" s="9">
@@ -2857,7 +4548,9 @@
       <c r="K57" t="n" s="12">
         <v>0.3298611111111111</v>
       </c>
-      <c r="L57"/>
+      <c r="L57" t="n" s="12">
+        <v>0.9798611111111111</v>
+      </c>
       <c r="M57" t="n" s="12">
         <v>0.9756944444444444</v>
       </c>
@@ -2884,7 +4577,7 @@
       <c r="C58" t="n" s="8">
         <v>58.0</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F58" t="s" s="120">
         <v>25</v>
       </c>
       <c r="G58" t="n" s="9">
@@ -2902,7 +4595,9 @@
       <c r="K58" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L58"/>
+      <c r="L58" t="n" s="12">
+        <v>0.9895833333333334</v>
+      </c>
       <c r="M58" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
@@ -2929,7 +4624,7 @@
       <c r="C59" t="n" s="8">
         <v>59.0</v>
       </c>
-      <c r="F59" t="s">
+      <c r="F59" t="s" s="122">
         <v>23</v>
       </c>
       <c r="G59" t="n" s="9">
@@ -2947,7 +4642,9 @@
       <c r="K59" t="n" s="12">
         <v>0.3020833333333333</v>
       </c>
-      <c r="L59"/>
+      <c r="L59" t="n" s="12">
+        <v>0.9986111111111111</v>
+      </c>
       <c r="M59" t="n" s="12">
         <v>0.9784722222222222</v>
       </c>
@@ -2974,7 +4671,7 @@
       <c r="C60" t="n" s="8">
         <v>60.0</v>
       </c>
-      <c r="F60" t="s">
+      <c r="F60" t="s" s="124">
         <v>23</v>
       </c>
       <c r="G60" t="n" s="9">
@@ -2992,7 +4689,9 @@
       <c r="K60" t="n" s="12">
         <v>0.2708333333333333</v>
       </c>
-      <c r="L60"/>
+      <c r="L60" t="n" s="12">
+        <v>0.9916666666666667</v>
+      </c>
       <c r="M60" t="n" s="12">
         <v>0.9833333333333333</v>
       </c>
@@ -3019,7 +4718,7 @@
       <c r="C61" t="n" s="8">
         <v>62.0</v>
       </c>
-      <c r="F61" t="s">
+      <c r="F61" t="s" s="126">
         <v>23</v>
       </c>
       <c r="G61" t="n" s="9">
@@ -3037,7 +4736,9 @@
       <c r="K61" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L61"/>
+      <c r="L61" t="n" s="12">
+        <v>0.99375</v>
+      </c>
       <c r="M61" t="n" s="12">
         <v>0.9881944444444445</v>
       </c>
@@ -3064,7 +4765,7 @@
       <c r="C62" t="n" s="8">
         <v>64.0</v>
       </c>
-      <c r="F62" t="s">
+      <c r="F62" t="s" s="128">
         <v>25</v>
       </c>
       <c r="G62" t="n" s="9">
@@ -3082,7 +4783,9 @@
       <c r="K62" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L62"/>
+      <c r="L62" t="n" s="12">
+        <v>0.9659722222222222</v>
+      </c>
       <c r="M62" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
@@ -3109,7 +4812,7 @@
       <c r="C63" t="n" s="8">
         <v>65.0</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" t="s" s="130">
         <v>23</v>
       </c>
       <c r="G63" t="n" s="9">
@@ -3127,7 +4830,9 @@
       <c r="K63" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L63"/>
+      <c r="L63" t="n" s="12">
+        <v>0.9583333333333334</v>
+      </c>
       <c r="M63" t="n" s="12">
         <v>0.9458333333333333</v>
       </c>
@@ -3154,7 +4859,7 @@
       <c r="C64" t="n" s="8">
         <v>67.0</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F64" t="s" s="132">
         <v>25</v>
       </c>
       <c r="G64" t="n" s="9">
@@ -3172,7 +4877,9 @@
       <c r="K64" t="n" s="12">
         <v>0.3229166666666667</v>
       </c>
-      <c r="L64"/>
+      <c r="L64" t="n" s="12">
+        <v>0.9368055555555556</v>
+      </c>
       <c r="M64" t="n" s="12">
         <v>0.9326388888888889</v>
       </c>
@@ -3199,7 +4906,7 @@
       <c r="C65" t="n" s="8">
         <v>68.0</v>
       </c>
-      <c r="F65" t="s">
+      <c r="F65" t="s" s="134">
         <v>23</v>
       </c>
       <c r="G65" t="n" s="9">
@@ -3217,7 +4924,9 @@
       <c r="K65" t="n" s="12">
         <v>0.3194444444444444</v>
       </c>
-      <c r="L65"/>
+      <c r="L65" t="n" s="12">
+        <v>0.9729166666666667</v>
+      </c>
       <c r="M65" t="n" s="12">
         <v>0.9625</v>
       </c>
@@ -3244,7 +4953,7 @@
       <c r="C66" t="n" s="8">
         <v>70.0</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" t="s" s="136">
         <v>24</v>
       </c>
       <c r="G66" t="n" s="9">
@@ -3262,7 +4971,9 @@
       <c r="K66" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L66"/>
+      <c r="L66" t="n" s="12">
+        <v>1.0027777777777778</v>
+      </c>
       <c r="M66" t="n" s="12">
         <v>0.9868055555555556</v>
       </c>
@@ -3289,7 +5000,7 @@
       <c r="C67" t="n" s="8">
         <v>71.0</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" t="s" s="138">
         <v>21</v>
       </c>
       <c r="G67" t="n" s="9">
@@ -3307,7 +5018,9 @@
       <c r="K67" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L67"/>
+      <c r="L67" t="n" s="12">
+        <v>0.9979166666666667</v>
+      </c>
       <c r="M67" t="n" s="12">
         <v>0.9881944444444445</v>
       </c>
@@ -3334,7 +5047,7 @@
       <c r="C68" t="n" s="8">
         <v>72.0</v>
       </c>
-      <c r="F68" t="s">
+      <c r="F68" t="s" s="140">
         <v>21</v>
       </c>
       <c r="G68" t="n" s="9">
@@ -3352,7 +5065,9 @@
       <c r="K68" t="n" s="12">
         <v>0.2708333333333333</v>
       </c>
-      <c r="L68"/>
+      <c r="L68" t="n" s="12">
+        <v>0.9791666666666666</v>
+      </c>
       <c r="M68" t="n" s="12">
         <v>0.9708333333333333</v>
       </c>
@@ -3379,7 +5094,7 @@
       <c r="C69" t="n" s="8">
         <v>73.0</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F69" t="s" s="142">
         <v>23</v>
       </c>
       <c r="G69" t="n" s="9">
@@ -3397,7 +5112,9 @@
       <c r="K69" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L69"/>
+      <c r="L69" t="n" s="12">
+        <v>0.9680555555555556</v>
+      </c>
       <c r="M69" t="n" s="12">
         <v>0.9625</v>
       </c>
@@ -3424,7 +5141,7 @@
       <c r="C70" t="n" s="8">
         <v>74.0</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F70" t="s" s="144">
         <v>23</v>
       </c>
       <c r="G70" t="n" s="9">
@@ -3442,7 +5159,9 @@
       <c r="K70" t="n" s="12">
         <v>0.2708333333333333</v>
       </c>
-      <c r="L70"/>
+      <c r="L70" t="n" s="12">
+        <v>0.9395833333333333</v>
+      </c>
       <c r="M70" t="n" s="12">
         <v>0.9375</v>
       </c>
@@ -3469,7 +5188,7 @@
       <c r="C71" t="n" s="8">
         <v>75.0</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F71" t="s" s="146">
         <v>23</v>
       </c>
       <c r="G71" t="n" s="9">
@@ -3487,7 +5206,9 @@
       <c r="K71" t="n" s="12">
         <v>0.2847222222222222</v>
       </c>
-      <c r="L71"/>
+      <c r="L71" t="n" s="12">
+        <v>0.9777777777777777</v>
+      </c>
       <c r="M71" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
@@ -3514,7 +5235,7 @@
       <c r="C72" t="n" s="8">
         <v>77.0</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F72" t="s" s="148">
         <v>23</v>
       </c>
       <c r="G72" t="n" s="9">
@@ -3532,7 +5253,9 @@
       <c r="K72" t="n" s="12">
         <v>0.2881944444444444</v>
       </c>
-      <c r="L72"/>
+      <c r="L72" t="n" s="12">
+        <v>0.9722222222222222</v>
+      </c>
       <c r="M72" t="n" s="12">
         <v>0.9618055555555556</v>
       </c>
@@ -3559,7 +5282,7 @@
       <c r="C73" t="n" s="8">
         <v>78.0</v>
       </c>
-      <c r="F73" t="s">
+      <c r="F73" t="s" s="150">
         <v>23</v>
       </c>
       <c r="G73" t="n" s="9">
@@ -3577,7 +5300,9 @@
       <c r="K73" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L73"/>
+      <c r="L73" t="n" s="12">
+        <v>0.9715277777777778</v>
+      </c>
       <c r="M73" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
@@ -3604,7 +5329,7 @@
       <c r="C74" t="n" s="8">
         <v>79.0</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F74" t="s" s="152">
         <v>24</v>
       </c>
       <c r="G74" t="n" s="9">
@@ -3622,7 +5347,9 @@
       <c r="K74" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L74"/>
+      <c r="L74" t="n" s="12">
+        <v>0.9673611111111111</v>
+      </c>
       <c r="M74" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
@@ -3649,7 +5376,7 @@
       <c r="C75" t="n" s="8">
         <v>80.0</v>
       </c>
-      <c r="F75" t="s">
+      <c r="F75" t="s" s="153">
         <v>20</v>
       </c>
       <c r="G75" t="n" s="9">
@@ -3667,7 +5394,9 @@
       <c r="K75" t="n" s="12">
         <v>0.3090277777777778</v>
       </c>
-      <c r="L75"/>
+      <c r="L75" t="n" s="12">
+        <v>0.9694444444444444</v>
+      </c>
       <c r="M75" t="n" s="12">
         <v>0.9604166666666667</v>
       </c>
@@ -3694,7 +5423,7 @@
       <c r="C76" t="n" s="8">
         <v>81.0</v>
       </c>
-      <c r="F76" t="s">
+      <c r="F76" t="s" s="155">
         <v>25</v>
       </c>
       <c r="G76" t="n" s="9">
@@ -3712,7 +5441,9 @@
       <c r="K76" t="n" s="12">
         <v>0.3333333333333333</v>
       </c>
-      <c r="L76"/>
+      <c r="L76" t="n" s="12">
+        <v>0.9319444444444445</v>
+      </c>
       <c r="M76" t="n" s="12">
         <v>0.9055555555555556</v>
       </c>
@@ -3739,7 +5470,7 @@
       <c r="C77" t="n" s="8">
         <v>82.0</v>
       </c>
-      <c r="F77" t="s">
+      <c r="F77" t="s" s="157">
         <v>25</v>
       </c>
       <c r="G77" t="n" s="9">
@@ -3757,7 +5488,9 @@
       <c r="K77" t="n" s="12">
         <v>0.3020833333333333</v>
       </c>
-      <c r="L77"/>
+      <c r="L77" t="n" s="12">
+        <v>0.9458333333333333</v>
+      </c>
       <c r="M77" t="n" s="12">
         <v>0.9270833333333334</v>
       </c>
@@ -3784,7 +5517,7 @@
       <c r="C78" t="n" s="8">
         <v>84.0</v>
       </c>
-      <c r="F78" t="s">
+      <c r="F78" t="s" s="159">
         <v>23</v>
       </c>
       <c r="G78" t="n" s="9">
@@ -3802,7 +5535,9 @@
       <c r="K78" t="n" s="12">
         <v>0.30416666666666664</v>
       </c>
-      <c r="L78"/>
+      <c r="L78" t="n" s="12">
+        <v>0.9944444444444445</v>
+      </c>
       <c r="M78" t="n" s="12">
         <v>0.9840277777777777</v>
       </c>
@@ -3829,7 +5564,7 @@
       <c r="C79" t="n" s="8">
         <v>86.0</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F79" t="s" s="161">
         <v>22</v>
       </c>
       <c r="G79" t="n" s="9">
@@ -3847,7 +5582,9 @@
       <c r="K79" t="n" s="12">
         <v>0.2951388888888889</v>
       </c>
-      <c r="L79"/>
+      <c r="L79" t="n" s="12">
+        <v>0.9993055555555556</v>
+      </c>
       <c r="M79" t="n" s="12">
         <v>0.9840277777777777</v>
       </c>
@@ -3874,7 +5611,7 @@
       <c r="C80" t="n" s="8">
         <v>87.0</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" t="s" s="163">
         <v>24</v>
       </c>
       <c r="G80" t="n" s="9">
@@ -3892,7 +5629,9 @@
       <c r="K80" t="n" s="12">
         <v>0.29583333333333334</v>
       </c>
-      <c r="L80"/>
+      <c r="L80" t="n" s="12">
+        <v>0.9972222222222222</v>
+      </c>
       <c r="M80" t="n" s="12">
         <v>0.98125</v>
       </c>
@@ -3919,7 +5658,7 @@
       <c r="C81" t="n" s="8">
         <v>88.0</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" t="s" s="165">
         <v>24</v>
       </c>
       <c r="G81" t="n" s="9">
@@ -3937,7 +5676,9 @@
       <c r="K81" t="n" s="12">
         <v>0.2777777777777778</v>
       </c>
-      <c r="L81"/>
+      <c r="L81" t="n" s="12">
+        <v>0.9972222222222222</v>
+      </c>
       <c r="M81" t="n" s="12">
         <v>0.9805555555555555</v>
       </c>
@@ -3964,7 +5705,7 @@
       <c r="C82" t="n" s="8">
         <v>89.0</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" t="s" s="167">
         <v>23</v>
       </c>
       <c r="G82" t="n" s="9">
@@ -3982,7 +5723,9 @@
       <c r="K82" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L82"/>
+      <c r="L82" t="n" s="12">
+        <v>0.9722222222222222</v>
+      </c>
       <c r="M82" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
@@ -4009,7 +5752,7 @@
       <c r="C83" t="n" s="8">
         <v>90.0</v>
       </c>
-      <c r="F83" t="s">
+      <c r="F83" t="s" s="169">
         <v>23</v>
       </c>
       <c r="G83" t="n" s="9">
@@ -4027,7 +5770,9 @@
       <c r="K83" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L83"/>
+      <c r="L83" t="n" s="12">
+        <v>0.9930555555555556</v>
+      </c>
       <c r="M83" t="n" s="12">
         <v>0.9729166666666667</v>
       </c>
@@ -4054,7 +5799,7 @@
       <c r="C84" t="n" s="8">
         <v>91.0</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F84" t="s" s="171">
         <v>25</v>
       </c>
       <c r="G84" t="n" s="9">
@@ -4072,7 +5817,9 @@
       <c r="K84" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L84"/>
+      <c r="L84" t="n" s="12">
+        <v>0.9826388888888888</v>
+      </c>
       <c r="M84" t="n" s="12">
         <v>0.9666666666666667</v>
       </c>
@@ -4099,7 +5846,7 @@
       <c r="C85" t="n" s="8">
         <v>92.0</v>
       </c>
-      <c r="F85" t="s">
+      <c r="F85" t="s" s="173">
         <v>25</v>
       </c>
       <c r="G85" t="n" s="9">
@@ -4117,7 +5864,9 @@
       <c r="K85" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L85"/>
+      <c r="L85" t="n" s="12">
+        <v>0.99375</v>
+      </c>
       <c r="M85" t="n" s="12">
         <v>0.9791666666666666</v>
       </c>
@@ -4144,7 +5893,7 @@
       <c r="C86" t="n" s="8">
         <v>94.0</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F86" t="s" s="175">
         <v>24</v>
       </c>
       <c r="G86" t="n" s="9">
@@ -4162,7 +5911,9 @@
       <c r="K86" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L86"/>
+      <c r="L86" t="n" s="12">
+        <v>0.975</v>
+      </c>
       <c r="M86" t="n" s="12">
         <v>0.9645833333333333</v>
       </c>
@@ -4189,7 +5940,7 @@
       <c r="C87" t="n" s="8">
         <v>95.0</v>
       </c>
-      <c r="F87" t="s">
+      <c r="F87" t="s" s="177">
         <v>24</v>
       </c>
       <c r="G87" t="n" s="9">
@@ -4207,7 +5958,9 @@
       <c r="K87" t="n" s="12">
         <v>0.2986111111111111</v>
       </c>
-      <c r="L87"/>
+      <c r="L87" t="n" s="12">
+        <v>1.0055555555555555</v>
+      </c>
       <c r="M87" t="n" s="12">
         <v>0.9958333333333333</v>
       </c>
@@ -4234,7 +5987,7 @@
       <c r="C88" t="n" s="8">
         <v>99.0</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F88" t="s" s="179">
         <v>23</v>
       </c>
       <c r="G88" t="n" s="9">
@@ -4252,7 +6005,9 @@
       <c r="K88" t="n" s="12">
         <v>0.2986111111111111</v>
       </c>
-      <c r="L88"/>
+      <c r="L88" t="n" s="12">
+        <v>0.9784722222222222</v>
+      </c>
       <c r="M88" t="n" s="12">
         <v>0.9652777777777778</v>
       </c>
@@ -4279,7 +6034,7 @@
       <c r="C89" t="n" s="8">
         <v>101.0</v>
       </c>
-      <c r="F89" t="s">
+      <c r="F89" t="s" s="181">
         <v>25</v>
       </c>
       <c r="G89" t="n" s="9">
@@ -4297,7 +6052,9 @@
       <c r="K89" t="n" s="12">
         <v>0.2972222222222222</v>
       </c>
-      <c r="L89"/>
+      <c r="L89" t="n" s="12">
+        <v>1.0125</v>
+      </c>
       <c r="M89" t="n" s="12">
         <v>1.0006944444444446</v>
       </c>
@@ -4324,7 +6081,7 @@
       <c r="C90" t="n" s="8">
         <v>102.0</v>
       </c>
-      <c r="F90" t="s">
+      <c r="F90" t="s" s="183">
         <v>25</v>
       </c>
       <c r="G90" t="n" s="9">
@@ -4342,7 +6099,9 @@
       <c r="K90" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L90"/>
+      <c r="L90" t="n" s="12">
+        <v>1.0215277777777778</v>
+      </c>
       <c r="M90" t="n" s="12">
         <v>0.9958333333333333</v>
       </c>
@@ -4369,7 +6128,7 @@
       <c r="C91" t="n" s="8">
         <v>103.0</v>
       </c>
-      <c r="F91" t="s">
+      <c r="F91" t="s" s="185">
         <v>23</v>
       </c>
       <c r="G91" t="n" s="9">
@@ -4387,7 +6146,9 @@
       <c r="K91" t="n" s="12">
         <v>0.2777777777777778</v>
       </c>
-      <c r="L91"/>
+      <c r="L91" t="n" s="12">
+        <v>0.98125</v>
+      </c>
       <c r="M91" t="n" s="12">
         <v>0.9701388888888889</v>
       </c>
@@ -4414,7 +6175,7 @@
       <c r="C92" t="n" s="8">
         <v>104.0</v>
       </c>
-      <c r="F92" t="s">
+      <c r="F92" t="s" s="187">
         <v>23</v>
       </c>
       <c r="G92" t="n" s="9">
@@ -4432,7 +6193,9 @@
       <c r="K92" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L92"/>
+      <c r="L92" t="n" s="12">
+        <v>0.9527777777777777</v>
+      </c>
       <c r="M92" t="n" s="12">
         <v>0.9479166666666666</v>
       </c>
@@ -4459,7 +6222,7 @@
       <c r="C93" t="n" s="8">
         <v>106.0</v>
       </c>
-      <c r="F93" t="s">
+      <c r="F93" t="s" s="189">
         <v>23</v>
       </c>
       <c r="G93" t="n" s="9">
@@ -4477,7 +6240,9 @@
       <c r="K93" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L93"/>
+      <c r="L93" t="n" s="12">
+        <v>1.0034722222222223</v>
+      </c>
       <c r="M93" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
@@ -4504,7 +6269,7 @@
       <c r="C94" t="n" s="8">
         <v>107.0</v>
       </c>
-      <c r="F94" t="s">
+      <c r="F94" t="s" s="191">
         <v>23</v>
       </c>
       <c r="G94" t="n" s="9">
@@ -4522,7 +6287,9 @@
       <c r="K94" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L94"/>
+      <c r="L94" t="n" s="12">
+        <v>0.9944444444444445</v>
+      </c>
       <c r="M94" t="n" s="12">
         <v>0.9826388888888888</v>
       </c>
@@ -4549,7 +6316,7 @@
       <c r="C95" t="n" s="8">
         <v>108.0</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F95" t="s" s="193">
         <v>23</v>
       </c>
       <c r="G95" t="n" s="9">
@@ -4567,7 +6334,9 @@
       <c r="K95" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L95"/>
+      <c r="L95" t="n" s="12">
+        <v>0.9930555555555556</v>
+      </c>
       <c r="M95" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
@@ -4594,7 +6363,7 @@
       <c r="C96" t="n" s="8">
         <v>109.0</v>
       </c>
-      <c r="F96" t="s">
+      <c r="F96" t="s" s="195">
         <v>25</v>
       </c>
       <c r="G96" t="n" s="9">
@@ -4612,7 +6381,9 @@
       <c r="K96" t="n" s="12">
         <v>0.3194444444444444</v>
       </c>
-      <c r="L96"/>
+      <c r="L96" t="n" s="12">
+        <v>0.9722222222222222</v>
+      </c>
       <c r="M96" t="n" s="12">
         <v>0.9666666666666667</v>
       </c>
@@ -4639,7 +6410,7 @@
       <c r="C97" t="n" s="8">
         <v>110.0</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F97" t="s" s="197">
         <v>23</v>
       </c>
       <c r="G97" t="n" s="9">
@@ -4657,7 +6428,9 @@
       <c r="K97" t="n" s="12">
         <v>0.3125</v>
       </c>
-      <c r="L97"/>
+      <c r="L97" t="n" s="12">
+        <v>0.9722222222222222</v>
+      </c>
       <c r="M97" t="n" s="12">
         <v>0.9583333333333334</v>
       </c>
@@ -4684,7 +6457,7 @@
       <c r="C98" t="n" s="8">
         <v>112.0</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F98" t="s" s="199">
         <v>23</v>
       </c>
       <c r="G98" t="n" s="9">
@@ -4702,7 +6475,9 @@
       <c r="K98" t="n" s="12">
         <v>0.2986111111111111</v>
       </c>
-      <c r="L98"/>
+      <c r="L98" t="n" s="12">
+        <v>0.9743055555555555</v>
+      </c>
       <c r="M98" t="n" s="12">
         <v>0.9631944444444445</v>
       </c>
@@ -4729,7 +6504,7 @@
       <c r="C99" t="n" s="8">
         <v>121.0</v>
       </c>
-      <c r="F99" t="s">
+      <c r="F99" t="s" s="201">
         <v>23</v>
       </c>
       <c r="G99" t="n" s="9">
@@ -4747,7 +6522,9 @@
       <c r="K99" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L99"/>
+      <c r="L99" t="n" s="12">
+        <v>0.9805555555555555</v>
+      </c>
       <c r="M99" t="n" s="12">
         <v>0.9756944444444444</v>
       </c>
@@ -4774,7 +6551,7 @@
       <c r="C100" t="n" s="8">
         <v>122.0</v>
       </c>
-      <c r="F100" t="s">
+      <c r="F100" t="s" s="203">
         <v>23</v>
       </c>
       <c r="G100" t="n" s="9">
@@ -4792,7 +6569,9 @@
       <c r="K100" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L100"/>
+      <c r="L100" t="n" s="12">
+        <v>0.9618055555555556</v>
+      </c>
       <c r="M100" t="n" s="12">
         <v>0.9479166666666666</v>
       </c>
@@ -4819,7 +6598,7 @@
       <c r="C101" t="n" s="8">
         <v>124.0</v>
       </c>
-      <c r="F101" t="s">
+      <c r="F101" t="s" s="205">
         <v>23</v>
       </c>
       <c r="G101" t="n" s="9">
@@ -4837,7 +6616,9 @@
       <c r="K101" t="n" s="12">
         <v>0.3541666666666667</v>
       </c>
-      <c r="L101"/>
+      <c r="L101" t="n" s="12">
+        <v>0.9902777777777778</v>
+      </c>
       <c r="M101" t="n" s="12">
         <v>0.9770833333333333</v>
       </c>
@@ -4864,7 +6645,7 @@
       <c r="C102" t="n" s="8">
         <v>150.0</v>
       </c>
-      <c r="F102" t="s">
+      <c r="F102" t="s" s="207">
         <v>24</v>
       </c>
       <c r="G102" t="n" s="9">
@@ -4882,7 +6663,9 @@
       <c r="K102" t="n" s="12">
         <v>0.2881944444444444</v>
       </c>
-      <c r="L102"/>
+      <c r="L102" t="n" s="12">
+        <v>0.9979166666666667</v>
+      </c>
       <c r="M102" t="n" s="12">
         <v>0.9826388888888888</v>
       </c>
@@ -4909,7 +6692,7 @@
       <c r="C103" t="n" s="8">
         <v>301.0</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F103" t="s" s="209">
         <v>22</v>
       </c>
       <c r="G103" t="n" s="9">
@@ -4927,7 +6710,9 @@
       <c r="K103" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L103"/>
+      <c r="L103" t="n" s="12">
+        <v>1.0347222222222223</v>
+      </c>
       <c r="M103" t="n" s="12">
         <v>1.011111111111111</v>
       </c>
@@ -4954,7 +6739,7 @@
       <c r="C104" t="n" s="8">
         <v>321.0</v>
       </c>
-      <c r="F104" t="s">
+      <c r="F104" t="s" s="211">
         <v>22</v>
       </c>
       <c r="G104" t="n" s="9">
@@ -4972,7 +6757,9 @@
       <c r="K104" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L104"/>
+      <c r="L104" t="n" s="12">
+        <v>0.9729166666666667</v>
+      </c>
       <c r="M104" t="n" s="12">
         <v>0.9652777777777778</v>
       </c>
@@ -4999,7 +6786,7 @@
       <c r="C105" t="n" s="8">
         <v>332.0</v>
       </c>
-      <c r="F105" t="s">
+      <c r="F105" t="s" s="213">
         <v>22</v>
       </c>
       <c r="G105" t="n" s="9">
@@ -5017,7 +6804,9 @@
       <c r="K105" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L105"/>
+      <c r="L105" t="n" s="12">
+        <v>1.0048611111111112</v>
+      </c>
       <c r="M105" t="n" s="12">
         <v>0.9861111111111112</v>
       </c>
@@ -5044,7 +6833,7 @@
       <c r="C106" t="n" s="8">
         <v>334.0</v>
       </c>
-      <c r="F106" t="s">
+      <c r="F106" t="s" s="215">
         <v>21</v>
       </c>
       <c r="G106" t="n" s="9">
@@ -5062,7 +6851,9 @@
       <c r="K106" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L106"/>
+      <c r="L106" t="n" s="12">
+        <v>0.9993055555555556</v>
+      </c>
       <c r="M106" t="n" s="12">
         <v>0.9729166666666667</v>
       </c>
@@ -5089,7 +6880,7 @@
       <c r="C107" t="n" s="8">
         <v>339.0</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F107" t="s" s="217">
         <v>22</v>
       </c>
       <c r="G107" t="n" s="9">
@@ -5107,7 +6898,9 @@
       <c r="K107" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L107"/>
+      <c r="L107" t="n" s="12">
+        <v>0.9791666666666666</v>
+      </c>
       <c r="M107" t="n" s="12">
         <v>0.9673611111111111</v>
       </c>
@@ -5134,7 +6927,7 @@
       <c r="C108" t="n" s="8">
         <v>343.0</v>
       </c>
-      <c r="F108" t="s">
+      <c r="F108" t="s" s="219">
         <v>22</v>
       </c>
       <c r="G108" t="n" s="9">
@@ -5152,7 +6945,9 @@
       <c r="K108" t="n" s="12">
         <v>0.2881944444444444</v>
       </c>
-      <c r="L108"/>
+      <c r="L108" t="n" s="12">
+        <v>1.020138888888889</v>
+      </c>
       <c r="M108" t="n" s="12">
         <v>0.9916666666666667</v>
       </c>
@@ -5179,7 +6974,7 @@
       <c r="C109" t="n" s="8">
         <v>344.0</v>
       </c>
-      <c r="F109" t="s">
+      <c r="F109" t="s" s="221">
         <v>22</v>
       </c>
       <c r="G109" t="n" s="9">
@@ -5197,7 +6992,9 @@
       <c r="K109" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L109"/>
+      <c r="L109" t="n" s="12">
+        <v>1.0027777777777778</v>
+      </c>
       <c r="M109" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
@@ -5224,7 +7021,7 @@
       <c r="C110" t="n" s="8">
         <v>345.0</v>
       </c>
-      <c r="F110" t="s">
+      <c r="F110" t="s" s="223">
         <v>22</v>
       </c>
       <c r="G110" t="n" s="9">
@@ -5242,7 +7039,9 @@
       <c r="K110" t="n" s="12">
         <v>0.2881944444444444</v>
       </c>
-      <c r="L110"/>
+      <c r="L110" t="n" s="12">
+        <v>1.0256944444444445</v>
+      </c>
       <c r="M110" t="n" s="12">
         <v>0.9930555555555556</v>
       </c>
@@ -5269,7 +7068,7 @@
       <c r="C111" t="n" s="8">
         <v>346.0</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F111" t="s" s="225">
         <v>22</v>
       </c>
       <c r="G111" t="n" s="9">
@@ -5287,7 +7086,9 @@
       <c r="K111" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L111"/>
+      <c r="L111" t="n" s="12">
+        <v>1.0208333333333333</v>
+      </c>
       <c r="M111" t="n" s="12">
         <v>0.9868055555555556</v>
       </c>
@@ -5314,7 +7115,7 @@
       <c r="C112" t="n" s="8">
         <v>363.0</v>
       </c>
-      <c r="F112" t="s">
+      <c r="F112" t="s" s="227">
         <v>23</v>
       </c>
       <c r="G112" t="n" s="9">
@@ -5332,7 +7133,9 @@
       <c r="K112" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L112"/>
+      <c r="L112" t="n" s="12">
+        <v>0.99375</v>
+      </c>
       <c r="M112" t="n" s="12">
         <v>0.9777777777777777</v>
       </c>
@@ -5359,7 +7162,7 @@
       <c r="C113" t="n" s="8">
         <v>383.0</v>
       </c>
-      <c r="F113" t="s">
+      <c r="F113" t="s" s="229">
         <v>23</v>
       </c>
       <c r="G113" t="n" s="9">
@@ -5377,7 +7180,9 @@
       <c r="K113" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L113"/>
+      <c r="L113" t="n" s="12">
+        <v>0.9986111111111111</v>
+      </c>
       <c r="M113" t="n" s="12">
         <v>0.9784722222222222</v>
       </c>
@@ -5404,7 +7209,7 @@
       <c r="C114" t="n" s="8">
         <v>385.0</v>
       </c>
-      <c r="F114" t="s">
+      <c r="F114" t="s" s="231">
         <v>22</v>
       </c>
       <c r="G114" t="n" s="9">
@@ -5422,7 +7227,9 @@
       <c r="K114" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L114"/>
+      <c r="L114" t="n" s="12">
+        <v>0.9875</v>
+      </c>
       <c r="M114" t="n" s="12">
         <v>0.9722222222222222</v>
       </c>
@@ -5449,7 +7256,7 @@
       <c r="C115" t="n" s="8">
         <v>387.0</v>
       </c>
-      <c r="F115" t="s">
+      <c r="F115" t="s" s="233">
         <v>22</v>
       </c>
       <c r="G115" t="n" s="9">
@@ -5467,7 +7274,9 @@
       <c r="K115" t="n" s="12">
         <v>0.2916666666666667</v>
       </c>
-      <c r="L115"/>
+      <c r="L115" t="n" s="12">
+        <v>0.9861111111111112</v>
+      </c>
       <c r="M115" t="n" s="12">
         <v>0.9701388888888889</v>
       </c>

</xml_diff>

<commit_message>
tripPeriod functions added (getTripPeriodTimeScheduledString, same for Actual, timeDifference and color
</commit_message>
<xml_diff>
--- a/downloads/sdasd.xlsx
+++ b/downloads/sdasd.xlsx
@@ -2727,67 +2727,67 @@
     </row>
     <row r="4">
       <c r="A4" t="n" s="5">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="B4" t="n" s="5">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="C4" t="n" s="5">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D4" t="n" s="5">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="E4" t="n" s="5">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="F4" t="n" s="5">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="G4" t="n" s="5">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="H4" t="n" s="5">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="I4" t="n" s="5">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="J4" t="n" s="5">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="K4" t="n" s="5">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="L4" t="n" s="5">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="M4" t="n" s="5">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="N4" t="n" s="5">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
       <c r="O4" t="n" s="5">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
       <c r="P4" t="n" s="5">
-        <v>15.0</v>
+        <v>16.0</v>
       </c>
       <c r="Q4" t="n" s="5">
-        <v>16.0</v>
+        <v>17.0</v>
       </c>
       <c r="R4" t="n" s="5">
-        <v>17.0</v>
+        <v>18.0</v>
       </c>
       <c r="S4" t="n" s="5">
-        <v>18.0</v>
+        <v>19.0</v>
       </c>
       <c r="T4" t="n" s="5">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
       <c r="U4" t="n" s="5">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="5" ht="30.0" customHeight="true">

</xml_diff>